<commit_message>
Updated Scrum Board with everyone's contributions.
</commit_message>
<xml_diff>
--- a/scrum board.xlsx
+++ b/scrum board.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="30" windowWidth="9570" windowHeight="8520"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Story</t>
   </si>
@@ -157,13 +157,37 @@
   </si>
   <si>
     <t>Jay</t>
+  </si>
+  <si>
+    <t>Created a splash screen for the application</t>
+  </si>
+  <si>
+    <t>Created edit texts and button for the login page</t>
+  </si>
+  <si>
+    <t>Created an onClickListener for the login page</t>
+  </si>
+  <si>
+    <t>Created a server application for the application to connect to</t>
+  </si>
+  <si>
+    <t>Added a command system in the server to check for command received by client</t>
+  </si>
+  <si>
+    <t>Implemented login command for the server (read user pass and return verification to client)</t>
+  </si>
+  <si>
+    <t>Implemented the login activity's onClickListener to talk to the server</t>
+  </si>
+  <si>
+    <t>Login activity receives whether or not a login was successful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,20 +219,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="3" tint="0.39997558519241921"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -230,13 +240,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -259,6 +262,20 @@
     <font>
       <sz val="12"/>
       <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -314,10 +331,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,17 +345,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,11 +655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +693,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -688,181 +702,252 @@
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>42</v>
+      <c r="F3" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C17" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="C14" s="9" t="s">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="C21" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="23" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="15" t="s">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="27" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="34" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="44" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+    <row r="45" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>